<commit_message>
account data table translation
</commit_message>
<xml_diff>
--- a/server/translations_for_ui.xlsx
+++ b/server/translations_for_ui.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="570" uniqueCount="381">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="571" uniqueCount="382">
   <si>
     <t>_name</t>
   </si>
@@ -935,6 +935,9 @@
   </si>
   <si>
     <t>电话</t>
+  </si>
+  <si>
+    <t>Phone</t>
   </si>
   <si>
     <t>Адрес доставки</t>
@@ -7071,9 +7074,8 @@
       <c r="C151" s="9" t="s">
         <v>307</v>
       </c>
-      <c r="D151" s="10" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(A151,""ru"",""en"")"),"Telephone")</f>
-        <v>Telephone</v>
+      <c r="D151" s="12" t="s">
+        <v>308</v>
       </c>
       <c r="E151" s="6"/>
       <c r="F151" s="6"/>
@@ -7100,13 +7102,13 @@
     </row>
     <row r="152">
       <c r="A152" s="7" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="B152" s="8" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="C152" s="9" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="D152" s="10" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(A152,""ru"",""en"")"),"Delivery address")</f>
@@ -7137,13 +7139,13 @@
     </row>
     <row r="153">
       <c r="A153" s="7" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="B153" s="8" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="C153" s="9" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="D153" s="10" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(A153,""ru"",""en"")"),"Account has been successfully edited!")</f>
@@ -7174,13 +7176,13 @@
     </row>
     <row r="154">
       <c r="A154" s="7" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="B154" s="8" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="C154" s="9" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="D154" s="10" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(A154,""ru"",""en"")"),"Goods are added to the basket!")</f>
@@ -7211,16 +7213,16 @@
     </row>
     <row r="155">
       <c r="A155" s="7" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="B155" s="8" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="C155" s="9" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="D155" s="13" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="E155" s="6"/>
       <c r="F155" s="6"/>
@@ -7247,13 +7249,13 @@
     </row>
     <row r="156">
       <c r="A156" s="7" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="B156" s="8" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="C156" s="9" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="D156" s="10" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(A156,""ru"",""en"")"),"Go to the basket")</f>
@@ -7284,13 +7286,13 @@
     </row>
     <row r="157">
       <c r="A157" s="7" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="B157" s="8" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="C157" s="9" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="D157" s="10" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(A157,""ru"",""en"")"),"Empty trash?")</f>
@@ -7321,13 +7323,13 @@
     </row>
     <row r="158">
       <c r="A158" s="7" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="B158" s="8" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="C158" s="9" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="D158" s="10" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(A158,""ru"",""en"")"),"Yes")</f>
@@ -7358,13 +7360,13 @@
     </row>
     <row r="159">
       <c r="A159" s="7" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="B159" s="8" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="C159" s="9" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="D159" s="10" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(A159,""ru"",""en"")"),"Price with VAT")</f>
@@ -7395,13 +7397,13 @@
     </row>
     <row r="160">
       <c r="A160" s="7" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="B160" s="8" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="C160" s="9" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="D160" s="10" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(A160,""ru"",""en"")"),"Price without VAT")</f>
@@ -7432,13 +7434,13 @@
     </row>
     <row r="161">
       <c r="A161" s="7" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="B161" s="8" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="C161" s="9" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="D161" s="10" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(A161,""ru"",""en"")"),"Price excluding VAT at the total order amount from 250 BYN")</f>
@@ -7469,13 +7471,13 @@
     </row>
     <row r="162">
       <c r="A162" s="7" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="B162" s="8" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="C162" s="9" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="D162" s="10" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(A162,""ru"",""en"")"),"Payment method:")</f>
@@ -7506,13 +7508,13 @@
     </row>
     <row r="163">
       <c r="A163" s="7" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="B163" s="8" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="C163" s="9" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="D163" s="10" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(A163,""ru"",""en"")"),"A comment")</f>
@@ -7543,13 +7545,13 @@
     </row>
     <row r="164">
       <c r="A164" s="7" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="B164" s="8" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="C164" s="9" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="D164" s="10" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(A164,""ru"",""en"")"),"Delivery:")</f>
@@ -7580,13 +7582,13 @@
     </row>
     <row r="165">
       <c r="A165" s="7" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="B165" s="8" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="C165" s="9" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="D165" s="10" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(A165,""ru"",""en"")"),"send")</f>
@@ -7617,13 +7619,13 @@
     </row>
     <row r="166">
       <c r="A166" s="7" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="B166" s="8" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="C166" s="9" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="D166" s="10" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(A166,""ru"",""en"")"),"Issue")</f>
@@ -7654,13 +7656,13 @@
     </row>
     <row r="167">
       <c r="A167" s="7" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="B167" s="8" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="C167" s="9" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="D167" s="10" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(A167,""ru"",""en"")"),"The order has been sent!")</f>
@@ -7691,13 +7693,13 @@
     </row>
     <row r="168">
       <c r="A168" s="7" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="B168" s="8" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="C168" s="9" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="D168" s="10" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(A168,""ru"",""en"")"),"Your room number")</f>
@@ -7728,13 +7730,13 @@
     </row>
     <row r="169">
       <c r="A169" s="7" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="B169" s="8" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="C169" s="9" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="D169" s="10" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(A169,""ru"",""en"")"),"Order confirmation sent to your email:")</f>
@@ -7765,13 +7767,13 @@
     </row>
     <row r="170">
       <c r="A170" s="7" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="B170" s="8" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="C170" s="9" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="D170" s="10" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(A170,""ru"",""en"")"),"In the near future, our manager will contact you to clarify the delivery details.")</f>
@@ -7802,13 +7804,13 @@
     </row>
     <row r="171">
       <c r="A171" s="7" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="B171" s="8" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="C171" s="9" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="D171" s="10" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(A171,""ru"",""en"")"),"An error has occurred!")</f>
@@ -7839,13 +7841,13 @@
     </row>
     <row r="172">
       <c r="A172" s="7" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="B172" s="8" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="C172" s="9" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="D172" s="10" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(A172,""ru"",""en"")"),"Your order is not sent")</f>
@@ -7876,13 +7878,13 @@
     </row>
     <row r="173">
       <c r="A173" s="7" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="B173" s="8" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="C173" s="9" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="D173" s="10" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(A173,""ru"",""en"")"),"Contact your support service or try later.")</f>
@@ -7913,13 +7915,13 @@
     </row>
     <row r="174">
       <c r="A174" s="7" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="B174" s="8" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="C174" s="9" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="D174" s="10" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(A174,""ru"",""en"")"),"Close")</f>
@@ -7950,13 +7952,13 @@
     </row>
     <row r="175">
       <c r="A175" s="7" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="B175" s="8" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="C175" s="9" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="D175" s="10" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(A175,""ru"",""en"")"),"Photo")</f>
@@ -7987,13 +7989,13 @@
     </row>
     <row r="176">
       <c r="A176" s="7" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="B176" s="8" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="C176" s="9" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="D176" s="10" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(A176,""ru"",""en"")"),"Name")</f>
@@ -8024,13 +8026,13 @@
     </row>
     <row r="177">
       <c r="A177" s="7" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="B177" s="8" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="C177" s="9" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="D177" s="10" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(A177,""ru"",""en"")"),"Count")</f>
@@ -8061,13 +8063,13 @@
     </row>
     <row r="178">
       <c r="A178" s="7" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="B178" s="8" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="C178" s="9" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="D178" s="10" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(A178,""ru"",""en"")"),"Price")</f>
@@ -8098,13 +8100,13 @@
     </row>
     <row r="179">
       <c r="A179" s="7" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="B179" s="8" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="C179" s="9" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="D179" s="10" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(A179,""ru"",""en"")"),"total amount")</f>
@@ -8135,13 +8137,13 @@
     </row>
     <row r="180">
       <c r="A180" s="7" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="B180" s="8" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="C180" s="9" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="D180" s="10" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(A180,""ru"",""en"")"),"Basket empty")</f>
@@ -8172,13 +8174,13 @@
     </row>
     <row r="181">
       <c r="A181" s="7" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="B181" s="8" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="C181" s="9" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="D181" s="10" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(A181,""ru"",""en"")"),"Password restored!")</f>
@@ -8209,13 +8211,13 @@
     </row>
     <row r="182">
       <c r="A182" s="7" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="B182" s="8" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="C182" s="9" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="D182" s="10" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(A182,""ru"",""en"")"),"The password is sent to you on email. Please check your mailbox.")</f>
@@ -8283,13 +8285,13 @@
     </row>
     <row r="184">
       <c r="A184" s="7" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="B184" s="8" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="C184" s="9" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="D184" s="10" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(A184,""ru"",""en"")"),"Order No.")</f>
@@ -8320,13 +8322,13 @@
     </row>
     <row r="185">
       <c r="A185" s="7" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="B185" s="8" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="C185" s="9" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="D185" s="10" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(A185,""ru"",""en"")"),"Repeat order")</f>
@@ -8357,13 +8359,13 @@
     </row>
     <row r="186">
       <c r="A186" s="7" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="B186" s="8" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="C186" s="9" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="D186" s="10" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(A186,""ru"",""en"")"),"No goods in this category")</f>
@@ -8394,13 +8396,13 @@
     </row>
     <row r="187">
       <c r="A187" s="7" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="B187" s="8" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="C187" s="9" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="D187" s="10" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(A187,""ru"",""en"")"),"show more")</f>

</xml_diff>

<commit_message>
account created modal translation
</commit_message>
<xml_diff>
--- a/server/translations_for_ui.xlsx
+++ b/server/translations_for_ui.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="600" uniqueCount="406">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="601" uniqueCount="407">
   <si>
     <t>_name</t>
   </si>
@@ -915,9 +915,6 @@
     <t>您的帐户</t>
   </si>
   <si>
-    <t>создан. Для входа используйте:</t>
-  </si>
-  <si>
     <t>创建。要登录，请使用：</t>
   </si>
   <si>
@@ -1237,6 +1234,12 @@
   </si>
   <si>
     <t>Soon, our manager will contact you to clarify the delivery details.</t>
+  </si>
+  <si>
+    <t>создан. Для входа используйте</t>
+  </si>
+  <si>
+    <t>created. Use:</t>
   </si>
 </sst>
 </file>
@@ -1645,8 +1648,8 @@
   </sheetPr>
   <dimension ref="A1:Z685"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A163" workbookViewId="0">
-      <selection activeCell="D170" sqref="D170"/>
+    <sheetView tabSelected="1" topLeftCell="A134" workbookViewId="0">
+      <selection activeCell="D147" sqref="D147"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1815,7 +1818,7 @@
         <v>12</v>
       </c>
       <c r="D5" s="10" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="E5" s="5"/>
       <c r="F5" s="6"/>
@@ -6511,7 +6514,7 @@
         <v>263</v>
       </c>
       <c r="D132" s="20" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="E132" s="6"/>
       <c r="F132" s="6"/>
@@ -7051,17 +7054,16 @@
     </row>
     <row r="147" spans="1:26" ht="15" x14ac:dyDescent="0.25">
       <c r="A147" s="7" t="s">
+        <v>405</v>
+      </c>
+      <c r="B147" s="8" t="s">
+        <v>405</v>
+      </c>
+      <c r="C147" s="9" t="s">
         <v>298</v>
       </c>
-      <c r="B147" s="8" t="s">
-        <v>298</v>
-      </c>
-      <c r="C147" s="9" t="s">
-        <v>299</v>
-      </c>
-      <c r="D147" s="10" t="str">
-        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(A147,""ru"",""en"")"),"Created. Use:")</f>
-        <v>Created. Use:</v>
+      <c r="D147" s="20" t="s">
+        <v>406</v>
       </c>
       <c r="E147" s="6"/>
       <c r="F147" s="6"/>
@@ -7088,13 +7090,13 @@
     </row>
     <row r="148" spans="1:26" ht="15" x14ac:dyDescent="0.25">
       <c r="A148" s="7" t="s">
+        <v>299</v>
+      </c>
+      <c r="B148" s="8" t="s">
+        <v>299</v>
+      </c>
+      <c r="C148" s="9" t="s">
         <v>300</v>
-      </c>
-      <c r="B148" s="8" t="s">
-        <v>300</v>
-      </c>
-      <c r="C148" s="9" t="s">
-        <v>301</v>
       </c>
       <c r="D148" s="10" t="str">
         <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(A148,""ru"",""en"")"),"Login")</f>
@@ -7125,13 +7127,13 @@
     </row>
     <row r="149" spans="1:26" ht="15" x14ac:dyDescent="0.25">
       <c r="A149" s="7" t="s">
+        <v>301</v>
+      </c>
+      <c r="B149" s="8" t="s">
+        <v>301</v>
+      </c>
+      <c r="C149" s="9" t="s">
         <v>302</v>
-      </c>
-      <c r="B149" s="8" t="s">
-        <v>302</v>
-      </c>
-      <c r="C149" s="9" t="s">
-        <v>303</v>
       </c>
       <c r="D149" s="10" t="str">
         <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(A149,""ru"",""en"")"),"Password")</f>
@@ -7162,13 +7164,13 @@
     </row>
     <row r="150" spans="1:26" ht="15" x14ac:dyDescent="0.25">
       <c r="A150" s="7" t="s">
+        <v>303</v>
+      </c>
+      <c r="B150" s="8" t="s">
+        <v>303</v>
+      </c>
+      <c r="C150" s="9" t="s">
         <v>304</v>
-      </c>
-      <c r="B150" s="8" t="s">
-        <v>304</v>
-      </c>
-      <c r="C150" s="9" t="s">
-        <v>305</v>
       </c>
       <c r="D150" s="10" t="str">
         <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(A150,""ru"",""en"")"),"Full name")</f>
@@ -7199,16 +7201,16 @@
     </row>
     <row r="151" spans="1:26" ht="15" x14ac:dyDescent="0.25">
       <c r="A151" s="7" t="s">
+        <v>305</v>
+      </c>
+      <c r="B151" s="8" t="s">
+        <v>305</v>
+      </c>
+      <c r="C151" s="9" t="s">
         <v>306</v>
       </c>
-      <c r="B151" s="8" t="s">
-        <v>306</v>
-      </c>
-      <c r="C151" s="9" t="s">
+      <c r="D151" s="12" t="s">
         <v>307</v>
-      </c>
-      <c r="D151" s="12" t="s">
-        <v>308</v>
       </c>
       <c r="E151" s="6"/>
       <c r="F151" s="6"/>
@@ -7235,13 +7237,13 @@
     </row>
     <row r="152" spans="1:26" ht="15" x14ac:dyDescent="0.25">
       <c r="A152" s="7" t="s">
+        <v>308</v>
+      </c>
+      <c r="B152" s="8" t="s">
+        <v>308</v>
+      </c>
+      <c r="C152" s="9" t="s">
         <v>309</v>
-      </c>
-      <c r="B152" s="8" t="s">
-        <v>309</v>
-      </c>
-      <c r="C152" s="9" t="s">
-        <v>310</v>
       </c>
       <c r="D152" s="10" t="str">
         <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(A152,""ru"",""en"")"),"Delivery address")</f>
@@ -7272,13 +7274,13 @@
     </row>
     <row r="153" spans="1:26" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A153" s="7" t="s">
+        <v>310</v>
+      </c>
+      <c r="B153" s="8" t="s">
+        <v>310</v>
+      </c>
+      <c r="C153" s="9" t="s">
         <v>311</v>
-      </c>
-      <c r="B153" s="8" t="s">
-        <v>311</v>
-      </c>
-      <c r="C153" s="9" t="s">
-        <v>312</v>
       </c>
       <c r="D153" s="10" t="str">
         <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(A153,""ru"",""en"")"),"Account has been successfully edited!")</f>
@@ -7309,13 +7311,13 @@
     </row>
     <row r="154" spans="1:26" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A154" s="7" t="s">
+        <v>312</v>
+      </c>
+      <c r="B154" s="8" t="s">
+        <v>312</v>
+      </c>
+      <c r="C154" s="9" t="s">
         <v>313</v>
-      </c>
-      <c r="B154" s="8" t="s">
-        <v>313</v>
-      </c>
-      <c r="C154" s="9" t="s">
-        <v>314</v>
       </c>
       <c r="D154" s="10" t="str">
         <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(A154,""ru"",""en"")"),"Goods are added to the basket!")</f>
@@ -7346,16 +7348,16 @@
     </row>
     <row r="155" spans="1:26" ht="51.75" x14ac:dyDescent="0.25">
       <c r="A155" s="7" t="s">
+        <v>314</v>
+      </c>
+      <c r="B155" s="8" t="s">
         <v>315</v>
       </c>
-      <c r="B155" s="8" t="s">
+      <c r="C155" s="9" t="s">
         <v>316</v>
       </c>
-      <c r="C155" s="9" t="s">
+      <c r="D155" s="13" t="s">
         <v>317</v>
-      </c>
-      <c r="D155" s="13" t="s">
-        <v>318</v>
       </c>
       <c r="E155" s="6"/>
       <c r="F155" s="6"/>
@@ -7382,13 +7384,13 @@
     </row>
     <row r="156" spans="1:26" ht="15" x14ac:dyDescent="0.25">
       <c r="A156" s="7" t="s">
+        <v>318</v>
+      </c>
+      <c r="B156" s="8" t="s">
+        <v>318</v>
+      </c>
+      <c r="C156" s="9" t="s">
         <v>319</v>
-      </c>
-      <c r="B156" s="8" t="s">
-        <v>319</v>
-      </c>
-      <c r="C156" s="9" t="s">
-        <v>320</v>
       </c>
       <c r="D156" s="10" t="str">
         <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(A156,""ru"",""en"")"),"Go to the basket")</f>
@@ -7419,13 +7421,13 @@
     </row>
     <row r="157" spans="1:26" ht="15" x14ac:dyDescent="0.25">
       <c r="A157" s="7" t="s">
+        <v>320</v>
+      </c>
+      <c r="B157" s="8" t="s">
+        <v>320</v>
+      </c>
+      <c r="C157" s="9" t="s">
         <v>321</v>
-      </c>
-      <c r="B157" s="8" t="s">
-        <v>321</v>
-      </c>
-      <c r="C157" s="9" t="s">
-        <v>322</v>
       </c>
       <c r="D157" s="10" t="str">
         <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(A157,""ru"",""en"")"),"Empty trash?")</f>
@@ -7456,13 +7458,13 @@
     </row>
     <row r="158" spans="1:26" ht="15" x14ac:dyDescent="0.25">
       <c r="A158" s="7" t="s">
+        <v>322</v>
+      </c>
+      <c r="B158" s="8" t="s">
+        <v>322</v>
+      </c>
+      <c r="C158" s="9" t="s">
         <v>323</v>
-      </c>
-      <c r="B158" s="8" t="s">
-        <v>323</v>
-      </c>
-      <c r="C158" s="9" t="s">
-        <v>324</v>
       </c>
       <c r="D158" s="10" t="str">
         <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(A158,""ru"",""en"")"),"Yes")</f>
@@ -7493,13 +7495,13 @@
     </row>
     <row r="159" spans="1:26" ht="15" x14ac:dyDescent="0.25">
       <c r="A159" s="7" t="s">
+        <v>324</v>
+      </c>
+      <c r="B159" s="8" t="s">
+        <v>324</v>
+      </c>
+      <c r="C159" s="9" t="s">
         <v>325</v>
-      </c>
-      <c r="B159" s="8" t="s">
-        <v>325</v>
-      </c>
-      <c r="C159" s="9" t="s">
-        <v>326</v>
       </c>
       <c r="D159" s="10" t="str">
         <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(A159,""ru"",""en"")"),"Price with VAT")</f>
@@ -7530,13 +7532,13 @@
     </row>
     <row r="160" spans="1:26" ht="15" x14ac:dyDescent="0.25">
       <c r="A160" s="7" t="s">
+        <v>326</v>
+      </c>
+      <c r="B160" s="8" t="s">
+        <v>326</v>
+      </c>
+      <c r="C160" s="9" t="s">
         <v>327</v>
-      </c>
-      <c r="B160" s="8" t="s">
-        <v>327</v>
-      </c>
-      <c r="C160" s="9" t="s">
-        <v>328</v>
       </c>
       <c r="D160" s="10" t="str">
         <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(A160,""ru"",""en"")"),"Price without VAT")</f>
@@ -7567,13 +7569,13 @@
     </row>
     <row r="161" spans="1:26" ht="39" x14ac:dyDescent="0.25">
       <c r="A161" s="7" t="s">
+        <v>328</v>
+      </c>
+      <c r="B161" s="8" t="s">
+        <v>328</v>
+      </c>
+      <c r="C161" s="9" t="s">
         <v>329</v>
-      </c>
-      <c r="B161" s="8" t="s">
-        <v>329</v>
-      </c>
-      <c r="C161" s="9" t="s">
-        <v>330</v>
       </c>
       <c r="D161" s="10" t="str">
         <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(A161,""ru"",""en"")"),"Price excluding VAT at the total order amount from 250 BYN")</f>
@@ -7604,13 +7606,13 @@
     </row>
     <row r="162" spans="1:26" ht="15" x14ac:dyDescent="0.25">
       <c r="A162" s="7" t="s">
+        <v>330</v>
+      </c>
+      <c r="B162" s="8" t="s">
+        <v>330</v>
+      </c>
+      <c r="C162" s="9" t="s">
         <v>331</v>
-      </c>
-      <c r="B162" s="8" t="s">
-        <v>331</v>
-      </c>
-      <c r="C162" s="9" t="s">
-        <v>332</v>
       </c>
       <c r="D162" s="10" t="str">
         <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(A162,""ru"",""en"")"),"Payment method:")</f>
@@ -7641,16 +7643,16 @@
     </row>
     <row r="163" spans="1:26" ht="15" x14ac:dyDescent="0.25">
       <c r="A163" s="7" t="s">
+        <v>332</v>
+      </c>
+      <c r="B163" s="8" t="s">
+        <v>332</v>
+      </c>
+      <c r="C163" s="9" t="s">
         <v>333</v>
       </c>
-      <c r="B163" s="8" t="s">
-        <v>333</v>
-      </c>
-      <c r="C163" s="9" t="s">
-        <v>334</v>
-      </c>
       <c r="D163" s="20" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="E163" s="6"/>
       <c r="F163" s="6"/>
@@ -7677,13 +7679,13 @@
     </row>
     <row r="164" spans="1:26" ht="15" x14ac:dyDescent="0.25">
       <c r="A164" s="7" t="s">
+        <v>334</v>
+      </c>
+      <c r="B164" s="8" t="s">
+        <v>334</v>
+      </c>
+      <c r="C164" s="9" t="s">
         <v>335</v>
-      </c>
-      <c r="B164" s="8" t="s">
-        <v>335</v>
-      </c>
-      <c r="C164" s="9" t="s">
-        <v>336</v>
       </c>
       <c r="D164" s="10" t="str">
         <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(A164,""ru"",""en"")"),"Delivery:")</f>
@@ -7714,16 +7716,16 @@
     </row>
     <row r="165" spans="1:26" ht="15" x14ac:dyDescent="0.25">
       <c r="A165" s="7" t="s">
+        <v>336</v>
+      </c>
+      <c r="B165" s="8" t="s">
+        <v>336</v>
+      </c>
+      <c r="C165" s="9" t="s">
         <v>337</v>
       </c>
-      <c r="B165" s="8" t="s">
-        <v>337</v>
-      </c>
-      <c r="C165" s="9" t="s">
-        <v>338</v>
-      </c>
       <c r="D165" s="10" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="E165" s="6"/>
       <c r="F165" s="6"/>
@@ -7750,16 +7752,16 @@
     </row>
     <row r="166" spans="1:26" ht="15" x14ac:dyDescent="0.25">
       <c r="A166" s="7" t="s">
+        <v>338</v>
+      </c>
+      <c r="B166" s="8" t="s">
+        <v>338</v>
+      </c>
+      <c r="C166" s="9" t="s">
         <v>339</v>
       </c>
-      <c r="B166" s="8" t="s">
-        <v>339</v>
-      </c>
-      <c r="C166" s="9" t="s">
-        <v>340</v>
-      </c>
       <c r="D166" s="10" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="E166" s="6"/>
       <c r="F166" s="6"/>
@@ -7786,13 +7788,13 @@
     </row>
     <row r="167" spans="1:26" ht="15" x14ac:dyDescent="0.25">
       <c r="A167" s="7" t="s">
+        <v>340</v>
+      </c>
+      <c r="B167" s="8" t="s">
+        <v>340</v>
+      </c>
+      <c r="C167" s="9" t="s">
         <v>341</v>
-      </c>
-      <c r="B167" s="8" t="s">
-        <v>341</v>
-      </c>
-      <c r="C167" s="9" t="s">
-        <v>342</v>
       </c>
       <c r="D167" s="10" t="str">
         <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(A167,""ru"",""en"")"),"The order has been sent!")</f>
@@ -7823,16 +7825,16 @@
     </row>
     <row r="168" spans="1:26" ht="15" x14ac:dyDescent="0.25">
       <c r="A168" s="7" t="s">
+        <v>342</v>
+      </c>
+      <c r="B168" s="8" t="s">
+        <v>342</v>
+      </c>
+      <c r="C168" s="9" t="s">
         <v>343</v>
       </c>
-      <c r="B168" s="8" t="s">
-        <v>343</v>
-      </c>
-      <c r="C168" s="9" t="s">
-        <v>344</v>
-      </c>
       <c r="D168" s="20" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="E168" s="6"/>
       <c r="F168" s="6"/>
@@ -7859,13 +7861,13 @@
     </row>
     <row r="169" spans="1:26" ht="30" x14ac:dyDescent="0.25">
       <c r="A169" s="7" t="s">
+        <v>344</v>
+      </c>
+      <c r="B169" s="8" t="s">
+        <v>344</v>
+      </c>
+      <c r="C169" s="9" t="s">
         <v>345</v>
-      </c>
-      <c r="B169" s="8" t="s">
-        <v>345</v>
-      </c>
-      <c r="C169" s="9" t="s">
-        <v>346</v>
       </c>
       <c r="D169" s="10" t="str">
         <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(A169,""ru"",""en"")"),"Order confirmation sent to your email:")</f>
@@ -7896,16 +7898,16 @@
     </row>
     <row r="170" spans="1:26" ht="39" x14ac:dyDescent="0.25">
       <c r="A170" s="7" t="s">
+        <v>346</v>
+      </c>
+      <c r="B170" s="8" t="s">
+        <v>346</v>
+      </c>
+      <c r="C170" s="9" t="s">
         <v>347</v>
       </c>
-      <c r="B170" s="8" t="s">
-        <v>347</v>
-      </c>
-      <c r="C170" s="9" t="s">
-        <v>348</v>
-      </c>
       <c r="D170" s="21" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="E170" s="6"/>
       <c r="F170" s="6"/>
@@ -7932,13 +7934,13 @@
     </row>
     <row r="171" spans="1:26" ht="15" x14ac:dyDescent="0.25">
       <c r="A171" s="7" t="s">
+        <v>348</v>
+      </c>
+      <c r="B171" s="8" t="s">
+        <v>348</v>
+      </c>
+      <c r="C171" s="9" t="s">
         <v>349</v>
-      </c>
-      <c r="B171" s="8" t="s">
-        <v>349</v>
-      </c>
-      <c r="C171" s="9" t="s">
-        <v>350</v>
       </c>
       <c r="D171" s="10" t="str">
         <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(A171,""ru"",""en"")"),"An error has occurred!")</f>
@@ -7969,13 +7971,13 @@
     </row>
     <row r="172" spans="1:26" ht="15" x14ac:dyDescent="0.25">
       <c r="A172" s="7" t="s">
+        <v>350</v>
+      </c>
+      <c r="B172" s="8" t="s">
+        <v>350</v>
+      </c>
+      <c r="C172" s="9" t="s">
         <v>351</v>
-      </c>
-      <c r="B172" s="8" t="s">
-        <v>351</v>
-      </c>
-      <c r="C172" s="9" t="s">
-        <v>352</v>
       </c>
       <c r="D172" s="10" t="str">
         <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(A172,""ru"",""en"")"),"Your order is not sent")</f>
@@ -8006,13 +8008,13 @@
     </row>
     <row r="173" spans="1:26" ht="30" x14ac:dyDescent="0.25">
       <c r="A173" s="7" t="s">
+        <v>352</v>
+      </c>
+      <c r="B173" s="8" t="s">
+        <v>352</v>
+      </c>
+      <c r="C173" s="9" t="s">
         <v>353</v>
-      </c>
-      <c r="B173" s="8" t="s">
-        <v>353</v>
-      </c>
-      <c r="C173" s="9" t="s">
-        <v>354</v>
       </c>
       <c r="D173" s="10" t="str">
         <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(A173,""ru"",""en"")"),"Contact your support service or try later.")</f>
@@ -8043,13 +8045,13 @@
     </row>
     <row r="174" spans="1:26" ht="15" x14ac:dyDescent="0.25">
       <c r="A174" s="7" t="s">
+        <v>354</v>
+      </c>
+      <c r="B174" s="8" t="s">
+        <v>354</v>
+      </c>
+      <c r="C174" s="9" t="s">
         <v>355</v>
-      </c>
-      <c r="B174" s="8" t="s">
-        <v>355</v>
-      </c>
-      <c r="C174" s="9" t="s">
-        <v>356</v>
       </c>
       <c r="D174" s="10" t="str">
         <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(A174,""ru"",""en"")"),"Close")</f>
@@ -8080,13 +8082,13 @@
     </row>
     <row r="175" spans="1:26" ht="15" x14ac:dyDescent="0.25">
       <c r="A175" s="7" t="s">
+        <v>356</v>
+      </c>
+      <c r="B175" s="8" t="s">
+        <v>356</v>
+      </c>
+      <c r="C175" s="9" t="s">
         <v>357</v>
-      </c>
-      <c r="B175" s="8" t="s">
-        <v>357</v>
-      </c>
-      <c r="C175" s="9" t="s">
-        <v>358</v>
       </c>
       <c r="D175" s="10" t="str">
         <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(A175,""ru"",""en"")"),"Photo")</f>
@@ -8117,13 +8119,13 @@
     </row>
     <row r="176" spans="1:26" ht="15" x14ac:dyDescent="0.25">
       <c r="A176" s="7" t="s">
+        <v>358</v>
+      </c>
+      <c r="B176" s="8" t="s">
+        <v>358</v>
+      </c>
+      <c r="C176" s="9" t="s">
         <v>359</v>
-      </c>
-      <c r="B176" s="8" t="s">
-        <v>359</v>
-      </c>
-      <c r="C176" s="9" t="s">
-        <v>360</v>
       </c>
       <c r="D176" s="10" t="str">
         <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(A176,""ru"",""en"")"),"Name")</f>
@@ -8154,13 +8156,13 @@
     </row>
     <row r="177" spans="1:26" ht="15" x14ac:dyDescent="0.25">
       <c r="A177" s="7" t="s">
+        <v>360</v>
+      </c>
+      <c r="B177" s="8" t="s">
+        <v>360</v>
+      </c>
+      <c r="C177" s="9" t="s">
         <v>361</v>
-      </c>
-      <c r="B177" s="8" t="s">
-        <v>361</v>
-      </c>
-      <c r="C177" s="9" t="s">
-        <v>362</v>
       </c>
       <c r="D177" s="10" t="str">
         <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(A177,""ru"",""en"")"),"Count")</f>
@@ -8191,13 +8193,13 @@
     </row>
     <row r="178" spans="1:26" ht="15" x14ac:dyDescent="0.25">
       <c r="A178" s="7" t="s">
+        <v>362</v>
+      </c>
+      <c r="B178" s="8" t="s">
+        <v>362</v>
+      </c>
+      <c r="C178" s="9" t="s">
         <v>363</v>
-      </c>
-      <c r="B178" s="8" t="s">
-        <v>363</v>
-      </c>
-      <c r="C178" s="9" t="s">
-        <v>364</v>
       </c>
       <c r="D178" s="10" t="str">
         <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(A178,""ru"",""en"")"),"Price")</f>
@@ -8228,16 +8230,16 @@
     </row>
     <row r="179" spans="1:26" ht="15" x14ac:dyDescent="0.25">
       <c r="A179" s="7" t="s">
+        <v>364</v>
+      </c>
+      <c r="B179" s="8" t="s">
+        <v>364</v>
+      </c>
+      <c r="C179" s="9" t="s">
         <v>365</v>
       </c>
-      <c r="B179" s="8" t="s">
-        <v>365</v>
-      </c>
-      <c r="C179" s="9" t="s">
-        <v>366</v>
-      </c>
       <c r="D179" s="20" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="E179" s="6"/>
       <c r="F179" s="6"/>
@@ -8264,13 +8266,13 @@
     </row>
     <row r="180" spans="1:26" ht="15" x14ac:dyDescent="0.25">
       <c r="A180" s="7" t="s">
+        <v>366</v>
+      </c>
+      <c r="B180" s="8" t="s">
+        <v>366</v>
+      </c>
+      <c r="C180" s="9" t="s">
         <v>367</v>
-      </c>
-      <c r="B180" s="8" t="s">
-        <v>367</v>
-      </c>
-      <c r="C180" s="9" t="s">
-        <v>368</v>
       </c>
       <c r="D180" s="10" t="str">
         <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(A180,""ru"",""en"")"),"Basket empty")</f>
@@ -8301,13 +8303,13 @@
     </row>
     <row r="181" spans="1:26" ht="15" x14ac:dyDescent="0.25">
       <c r="A181" s="7" t="s">
+        <v>368</v>
+      </c>
+      <c r="B181" s="8" t="s">
+        <v>368</v>
+      </c>
+      <c r="C181" s="9" t="s">
         <v>369</v>
-      </c>
-      <c r="B181" s="8" t="s">
-        <v>369</v>
-      </c>
-      <c r="C181" s="9" t="s">
-        <v>370</v>
       </c>
       <c r="D181" s="10" t="str">
         <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(A181,""ru"",""en"")"),"Password restored!")</f>
@@ -8338,13 +8340,13 @@
     </row>
     <row r="182" spans="1:26" ht="39" x14ac:dyDescent="0.25">
       <c r="A182" s="7" t="s">
+        <v>370</v>
+      </c>
+      <c r="B182" s="8" t="s">
         <v>371</v>
       </c>
-      <c r="B182" s="8" t="s">
+      <c r="C182" s="9" t="s">
         <v>372</v>
-      </c>
-      <c r="C182" s="9" t="s">
-        <v>373</v>
       </c>
       <c r="D182" s="10" t="str">
         <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(A182,""ru"",""en"")"),"The password is sent to you on email. Please check your mailbox.")</f>
@@ -8412,13 +8414,13 @@
     </row>
     <row r="184" spans="1:26" ht="15" x14ac:dyDescent="0.25">
       <c r="A184" s="19" t="s">
+        <v>373</v>
+      </c>
+      <c r="B184" s="8" t="s">
+        <v>373</v>
+      </c>
+      <c r="C184" s="9" t="s">
         <v>374</v>
-      </c>
-      <c r="B184" s="8" t="s">
-        <v>374</v>
-      </c>
-      <c r="C184" s="9" t="s">
-        <v>375</v>
       </c>
       <c r="D184" s="10" t="str">
         <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(A184,""ru"",""en"")"),"Order No.")</f>
@@ -8449,13 +8451,13 @@
     </row>
     <row r="185" spans="1:26" ht="15" x14ac:dyDescent="0.25">
       <c r="A185" s="7" t="s">
+        <v>375</v>
+      </c>
+      <c r="B185" s="8" t="s">
+        <v>375</v>
+      </c>
+      <c r="C185" s="9" t="s">
         <v>376</v>
-      </c>
-      <c r="B185" s="8" t="s">
-        <v>376</v>
-      </c>
-      <c r="C185" s="9" t="s">
-        <v>377</v>
       </c>
       <c r="D185" s="10" t="str">
         <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(A185,""ru"",""en"")"),"Repeat order")</f>
@@ -8486,13 +8488,13 @@
     </row>
     <row r="186" spans="1:26" ht="15" x14ac:dyDescent="0.25">
       <c r="A186" s="7" t="s">
+        <v>377</v>
+      </c>
+      <c r="B186" s="8" t="s">
+        <v>377</v>
+      </c>
+      <c r="C186" s="9" t="s">
         <v>378</v>
-      </c>
-      <c r="B186" s="8" t="s">
-        <v>378</v>
-      </c>
-      <c r="C186" s="9" t="s">
-        <v>379</v>
       </c>
       <c r="D186" s="10" t="str">
         <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(A186,""ru"",""en"")"),"No goods in this category")</f>
@@ -8523,16 +8525,16 @@
     </row>
     <row r="187" spans="1:26" ht="15" x14ac:dyDescent="0.25">
       <c r="A187" s="7" t="s">
+        <v>379</v>
+      </c>
+      <c r="B187" s="8" t="s">
+        <v>379</v>
+      </c>
+      <c r="C187" s="9" t="s">
         <v>380</v>
       </c>
-      <c r="B187" s="8" t="s">
-        <v>380</v>
-      </c>
-      <c r="C187" s="9" t="s">
+      <c r="D187" s="10" t="s">
         <v>381</v>
-      </c>
-      <c r="D187" s="10" t="s">
-        <v>382</v>
       </c>
       <c r="E187" s="6"/>
       <c r="F187" s="6"/>
@@ -8559,16 +8561,16 @@
     </row>
     <row r="188" spans="1:26" ht="15" x14ac:dyDescent="0.25">
       <c r="A188" s="7" t="s">
+        <v>382</v>
+      </c>
+      <c r="B188" s="8" t="s">
+        <v>382</v>
+      </c>
+      <c r="C188" s="9" t="s">
         <v>383</v>
       </c>
-      <c r="B188" s="8" t="s">
-        <v>383</v>
-      </c>
-      <c r="C188" s="9" t="s">
+      <c r="D188" s="10" t="s">
         <v>384</v>
-      </c>
-      <c r="D188" s="10" t="s">
-        <v>385</v>
       </c>
       <c r="E188" s="6"/>
       <c r="F188" s="6"/>
@@ -8595,16 +8597,16 @@
     </row>
     <row r="189" spans="1:26" ht="15" x14ac:dyDescent="0.25">
       <c r="A189" s="15" t="s">
+        <v>385</v>
+      </c>
+      <c r="B189" s="17" t="s">
+        <v>385</v>
+      </c>
+      <c r="C189" s="16" t="s">
         <v>386</v>
       </c>
-      <c r="B189" s="17" t="s">
-        <v>386</v>
-      </c>
-      <c r="C189" s="16" t="s">
+      <c r="D189" s="18" t="s">
         <v>387</v>
-      </c>
-      <c r="D189" s="18" t="s">
-        <v>388</v>
       </c>
       <c r="E189" s="6"/>
       <c r="F189" s="6"/>
@@ -8631,16 +8633,16 @@
     </row>
     <row r="190" spans="1:26" ht="15" x14ac:dyDescent="0.25">
       <c r="A190" s="15" t="s">
+        <v>393</v>
+      </c>
+      <c r="B190" s="17" t="s">
+        <v>393</v>
+      </c>
+      <c r="C190" s="16" t="s">
         <v>394</v>
       </c>
-      <c r="B190" s="17" t="s">
-        <v>394</v>
-      </c>
-      <c r="C190" s="16" t="s">
+      <c r="D190" s="18" t="s">
         <v>395</v>
-      </c>
-      <c r="D190" s="18" t="s">
-        <v>396</v>
       </c>
       <c r="E190" s="6"/>
       <c r="F190" s="6"/>
@@ -8667,16 +8669,16 @@
     </row>
     <row r="191" spans="1:26" ht="15" x14ac:dyDescent="0.25">
       <c r="A191" s="15" t="s">
+        <v>396</v>
+      </c>
+      <c r="B191" s="17" t="s">
+        <v>396</v>
+      </c>
+      <c r="C191" s="16" t="s">
         <v>397</v>
       </c>
-      <c r="B191" s="17" t="s">
-        <v>397</v>
-      </c>
-      <c r="C191" s="16" t="s">
+      <c r="D191" s="18" t="s">
         <v>398</v>
-      </c>
-      <c r="D191" s="18" t="s">
-        <v>399</v>
       </c>
       <c r="E191" s="6"/>
       <c r="F191" s="6"/>
@@ -8703,16 +8705,16 @@
     </row>
     <row r="192" spans="1:26" ht="15" x14ac:dyDescent="0.25">
       <c r="A192" s="15" t="s">
+        <v>399</v>
+      </c>
+      <c r="B192" s="17" t="s">
+        <v>399</v>
+      </c>
+      <c r="C192" s="16" t="s">
         <v>400</v>
       </c>
-      <c r="B192" s="17" t="s">
-        <v>400</v>
-      </c>
-      <c r="C192" s="16" t="s">
+      <c r="D192" s="18" t="s">
         <v>401</v>
-      </c>
-      <c r="D192" s="18" t="s">
-        <v>402</v>
       </c>
       <c r="E192" s="6"/>
       <c r="F192" s="6"/>

</xml_diff>

<commit_message>
add history to cart modal
</commit_message>
<xml_diff>
--- a/server/translations_for_ui.xlsx
+++ b/server/translations_for_ui.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="601" uniqueCount="407">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="604" uniqueCount="410">
   <si>
     <t>_name</t>
   </si>
@@ -1240,6 +1240,15 @@
   </si>
   <si>
     <t>created. Use:</t>
+  </si>
+  <si>
+    <t>Cart is empty</t>
+  </si>
+  <si>
+    <t>Goods are added to the cart!</t>
+  </si>
+  <si>
+    <t>Go to the cart</t>
   </si>
 </sst>
 </file>
@@ -1648,8 +1657,8 @@
   </sheetPr>
   <dimension ref="A1:Z685"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A134" workbookViewId="0">
-      <selection activeCell="D147" sqref="D147"/>
+    <sheetView tabSelected="1" topLeftCell="A149" workbookViewId="0">
+      <selection activeCell="D158" sqref="D158"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -7309,7 +7318,7 @@
       <c r="Y153" s="6"/>
       <c r="Z153" s="6"/>
     </row>
-    <row r="154" spans="1:26" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:26" ht="15" x14ac:dyDescent="0.25">
       <c r="A154" s="7" t="s">
         <v>312</v>
       </c>
@@ -7319,9 +7328,8 @@
       <c r="C154" s="9" t="s">
         <v>313</v>
       </c>
-      <c r="D154" s="10" t="str">
-        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(A154,""ru"",""en"")"),"Goods are added to the basket!")</f>
-        <v>Goods are added to the basket!</v>
+      <c r="D154" s="20" t="s">
+        <v>408</v>
       </c>
       <c r="E154" s="6"/>
       <c r="F154" s="6"/>
@@ -7392,9 +7400,8 @@
       <c r="C156" s="9" t="s">
         <v>319</v>
       </c>
-      <c r="D156" s="10" t="str">
-        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(A156,""ru"",""en"")"),"Go to the basket")</f>
-        <v>Go to the basket</v>
+      <c r="D156" s="20" t="s">
+        <v>409</v>
       </c>
       <c r="E156" s="6"/>
       <c r="F156" s="6"/>
@@ -8274,9 +8281,8 @@
       <c r="C180" s="9" t="s">
         <v>367</v>
       </c>
-      <c r="D180" s="10" t="str">
-        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(A180,""ru"",""en"")"),"Basket empty")</f>
-        <v>Basket empty</v>
+      <c r="D180" s="10" t="s">
+        <v>407</v>
       </c>
       <c r="E180" s="6"/>
       <c r="F180" s="6"/>

</xml_diff>

<commit_message>
fix chat button close clean cart button
</commit_message>
<xml_diff>
--- a/server/translations_for_ui.xlsx
+++ b/server/translations_for_ui.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="716" uniqueCount="494">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="728" uniqueCount="503">
   <si>
     <t>_name</t>
   </si>
@@ -1493,6 +1493,33 @@
   </si>
   <si>
     <t>Remove item from the cart?</t>
+  </si>
+  <si>
+    <t>Показывать только товары в наличии</t>
+  </si>
+  <si>
+    <t>仅显示库存商品</t>
+  </si>
+  <si>
+    <t>Show only goods in stock</t>
+  </si>
+  <si>
+    <t>Чат</t>
+  </si>
+  <si>
+    <t>聊天</t>
+  </si>
+  <si>
+    <t>Chat</t>
+  </si>
+  <si>
+    <t>Ничего не найдено. Попробуйте изменить поисковый запрос.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">什么都没找到。 请尝试更改搜索请求 </t>
+  </si>
+  <si>
+    <t>Nothing found. Please try to change search request</t>
   </si>
 </sst>
 </file>
@@ -6612,8 +6639,8 @@
         <v>258</v>
       </c>
       <c r="D129" s="10" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(A129,""ru"",""en"")"),"To main")</f>
-        <v>To main</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(A129,""ru"",""en"")"),"To the main")</f>
+        <v>To the main</v>
       </c>
       <c r="E129" s="6"/>
       <c r="F129" s="6"/>
@@ -6649,8 +6676,8 @@
         <v>260</v>
       </c>
       <c r="D130" s="10" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(A130,""ru"",""en"")"),"Exit")</f>
-        <v>Exit</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(A130,""ru"",""en"")"),"Output")</f>
+        <v>Output</v>
       </c>
       <c r="E130" s="6"/>
       <c r="F130" s="6"/>
@@ -7014,8 +7041,8 @@
         <v>286</v>
       </c>
       <c r="D140" s="10" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(A140,""ru"",""en"")"),"Error")</f>
-        <v>Error</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(A140,""ru"",""en"")"),"Mistake")</f>
+        <v>Mistake</v>
       </c>
       <c r="E140" s="6"/>
       <c r="F140" s="6"/>
@@ -8298,8 +8325,8 @@
         <v>368</v>
       </c>
       <c r="D175" s="10" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(A175,""ru"",""en"")"),"Photo")</f>
-        <v>Photo</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(A175,""ru"",""en"")"),"A photo")</f>
+        <v>A photo</v>
       </c>
       <c r="E175" s="6"/>
       <c r="F175" s="6"/>
@@ -8592,8 +8619,8 @@
         <v>258</v>
       </c>
       <c r="D183" s="10" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(A183,""ru"",""en"")"),"To main")</f>
-        <v>To main</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(A183,""ru"",""en"")"),"To the main")</f>
+        <v>To the main</v>
       </c>
       <c r="E183" s="6"/>
       <c r="F183" s="6"/>
@@ -9954,10 +9981,18 @@
       <c r="Z220" s="6"/>
     </row>
     <row r="221">
-      <c r="A221" s="16"/>
-      <c r="B221" s="16"/>
-      <c r="C221" s="17"/>
-      <c r="D221" s="18"/>
+      <c r="A221" s="16" t="s">
+        <v>494</v>
+      </c>
+      <c r="B221" s="16" t="s">
+        <v>494</v>
+      </c>
+      <c r="C221" s="17" t="s">
+        <v>495</v>
+      </c>
+      <c r="D221" s="18" t="s">
+        <v>496</v>
+      </c>
       <c r="E221" s="6"/>
       <c r="F221" s="6"/>
       <c r="G221" s="6"/>
@@ -9982,10 +10017,18 @@
       <c r="Z221" s="6"/>
     </row>
     <row r="222">
-      <c r="A222" s="16"/>
-      <c r="B222" s="16"/>
-      <c r="C222" s="17"/>
-      <c r="D222" s="18"/>
+      <c r="A222" s="16" t="s">
+        <v>497</v>
+      </c>
+      <c r="B222" s="16" t="s">
+        <v>497</v>
+      </c>
+      <c r="C222" s="17" t="s">
+        <v>498</v>
+      </c>
+      <c r="D222" s="18" t="s">
+        <v>499</v>
+      </c>
       <c r="E222" s="6"/>
       <c r="F222" s="6"/>
       <c r="G222" s="6"/>
@@ -10010,10 +10053,18 @@
       <c r="Z222" s="6"/>
     </row>
     <row r="223">
-      <c r="A223" s="16"/>
-      <c r="B223" s="16"/>
-      <c r="C223" s="17"/>
-      <c r="D223" s="18"/>
+      <c r="A223" s="16" t="s">
+        <v>500</v>
+      </c>
+      <c r="B223" s="16" t="s">
+        <v>500</v>
+      </c>
+      <c r="C223" s="17" t="s">
+        <v>501</v>
+      </c>
+      <c r="D223" s="18" t="s">
+        <v>502</v>
+      </c>
       <c r="E223" s="6"/>
       <c r="F223" s="6"/>
       <c r="G223" s="6"/>

</xml_diff>